<commit_message>
FD : Ajout de l'excel avec les aptitudes, et autres
</commit_message>
<xml_diff>
--- a/docs/lieux.xlsx
+++ b/docs/lieux.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC-CDA-12\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CDA-08\Desktop\projet\jdr2d\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1024B5-A77C-4FD7-B7B7-FFBF5701CA94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7002CD3-729E-4B13-9311-7B45D9F174DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EAFB9A12-5683-4B08-B3E7-0ACF3A3D935D}"/>
+    <workbookView xWindow="31230" yWindow="1410" windowWidth="21600" windowHeight="11385" xr2:uid="{EAFB9A12-5683-4B08-B3E7-0ACF3A3D935D}"/>
   </bookViews>
   <sheets>
     <sheet name="Lieux-PnJ" sheetId="1" r:id="rId1"/>
@@ -1189,6 +1189,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1211,63 +1268,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1587,403 +1587,403 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="15" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.5703125" style="15" customWidth="1"/>
-    <col min="7" max="7" width="24" style="15" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17" style="15" customWidth="1"/>
-    <col min="11" max="11" width="19.7109375" style="15" customWidth="1"/>
-    <col min="12" max="16384" width="11.42578125" style="15"/>
+    <col min="1" max="1" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.5703125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="24" style="7" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" style="7" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" style="7" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="8" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="10"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="29"/>
       <c r="E2" s="1"/>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="11" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="22"/>
+      <c r="C3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="16" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="21" t="s">
+      <c r="B4" s="22"/>
+      <c r="C4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="18"/>
+      <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="21" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="18"/>
+      <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="21" t="s">
+      <c r="B6" s="23"/>
+      <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="27"/>
       <c r="E7" s="2"/>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="21" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="14" t="s">
         <v>61</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="21" t="s">
+      <c r="B9" s="22"/>
+      <c r="C9" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="21" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="14" t="s">
         <v>91</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="21" t="s">
+      <c r="B11" s="23"/>
+      <c r="C11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="8"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="27"/>
       <c r="E12" s="2"/>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="21" t="s">
+      <c r="B13" s="22"/>
+      <c r="C13" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="G13" s="25" t="s">
+      <c r="G13" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="21" t="s">
+      <c r="B14" s="22"/>
+      <c r="C14" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="15" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="21" t="s">
+      <c r="B15" s="22"/>
+      <c r="C15" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="14" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="21" t="s">
+      <c r="B16" s="23"/>
+      <c r="C16" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="E16" s="23" t="s">
+      <c r="E16" s="15" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="8"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="27"/>
       <c r="E17" s="2"/>
-      <c r="I17" s="15" t="s">
+      <c r="I17" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="21" t="s">
+      <c r="B18" s="22"/>
+      <c r="C18" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="14" t="s">
         <v>67</v>
       </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="21" t="s">
+      <c r="B19" s="22"/>
+      <c r="C19" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="15" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="21" t="s">
+      <c r="B20" s="22"/>
+      <c r="C20" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D20" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="E20" s="15" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="27" t="s">
+      <c r="B21" s="25"/>
+      <c r="C21" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="21" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>